<commit_message>
Updating files for a general version (v02)
</commit_message>
<xml_diff>
--- a/Excel_Results/YX_C pH_UL.xlsx
+++ b/Excel_Results/YX_C pH_UL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY4"/>
+  <dimension ref="A1:AM3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,72 +621,12 @@
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>t_value_k_C</t>
+          <t>t_value_YX_C</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>t_value_k_N</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>t_value_k_O</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>t_value_k_d</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>t_value_YX_CO2</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>t_value_YX_O2</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>t_value_YX_C</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>t_value_YX_N</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
-        <is>
-          <t>t_value_Xmax</t>
-        </is>
-      </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>t_value_mu_max</t>
-        </is>
-      </c>
-      <c r="AV1" s="1" t="inlineStr">
-        <is>
-          <t>t_value_pH_LL</t>
-        </is>
-      </c>
-      <c r="AW1" s="1" t="inlineStr">
-        <is>
           <t>t_value_pH_UL</t>
-        </is>
-      </c>
-      <c r="AX1" s="1" t="inlineStr">
-        <is>
-          <t>t_value_I_val</t>
-        </is>
-      </c>
-      <c r="AY1" s="1" t="inlineStr">
-        <is>
-          <t>t_value_O2_sat</t>
         </is>
       </c>
     </row>
@@ -772,30 +712,18 @@
       <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="inlineStr"/>
-      <c r="AN2" t="inlineStr"/>
-      <c r="AO2" t="inlineStr"/>
-      <c r="AP2" t="inlineStr"/>
-      <c r="AQ2" t="inlineStr"/>
-      <c r="AR2" t="inlineStr"/>
-      <c r="AS2" t="inlineStr"/>
-      <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="inlineStr"/>
-      <c r="AV2" t="inlineStr"/>
-      <c r="AW2" t="inlineStr"/>
-      <c r="AX2" t="inlineStr"/>
-      <c r="AY2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Run_2</t>
+          <t>Run_3</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.111276868937633</v>
+        <v>0.3019000248478971</v>
       </c>
       <c r="C3" t="n">
-        <v>6.308552868952525</v>
+        <v>6.270094823160237</v>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -815,197 +743,62 @@
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
-        <v>0.1497157199646922</v>
+        <v>0.1767723542181233</v>
       </c>
       <c r="V3" t="n">
-        <v>0.1526168129622923</v>
+        <v>0.1801977329232616</v>
       </c>
       <c r="W3" t="n">
-        <v>16.96903091182692</v>
+        <v>21.53459878428799</v>
       </c>
       <c r="X3" t="n">
-        <v>0.8686244496617416</v>
+        <v>1.288233347656097</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.3812320199235195</v>
+        <v>0.5653948624759768</v>
       </c>
       <c r="Z3" t="n">
-        <v>18.37064359640591</v>
+        <v>27.81498117706033</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.0604853173443286</v>
+        <v>0.05908581434424913</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.4768240174593737</v>
+        <v>0.4657913127924631</v>
       </c>
       <c r="AC3" t="n">
-        <v>6.074796290562643</v>
+        <v>5.922211725760993</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.06235633742473321</v>
+        <v>0.0780941576563732</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.07893207268953571</v>
+        <v>0.09885336412199139</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.7468641188818747</v>
+        <v>0.9373952689530096</v>
       </c>
       <c r="AG3" t="n">
-        <v>-56.64548632859142</v>
+        <v>-28.79586067230095</v>
       </c>
       <c r="AH3" t="n">
-        <v>-55.06196739013531</v>
+        <v>-27.21234173384484</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.4428515602845892</v>
+        <v>0.6519937603508629</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.06362517854083935</v>
+        <v>0.0936729665876723</v>
       </c>
       <c r="AK3" t="n">
-        <v>10.54033372941934</v>
+        <v>14.05229673901558</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.3117698520820912</v>
+        <v>650.6571407306653</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.131093784906223</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0.1542149950110357</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>6.898559769911134</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>468.8982638860226</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>6.096885929964035</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>152.516685661391</v>
-      </c>
-      <c r="AS3" t="n">
-        <v>264.4236610596811</v>
-      </c>
-      <c r="AT3" t="n">
-        <v>249.6488232148385</v>
-      </c>
-      <c r="AU3" t="n">
-        <v>2.17400201450181</v>
-      </c>
-      <c r="AV3" t="n">
-        <v>50.87987774245172</v>
-      </c>
-      <c r="AW3" t="n">
-        <v>147.61558856492</v>
-      </c>
-      <c r="AX3" t="n">
-        <v>10.37950270080371</v>
-      </c>
-      <c r="AY3" t="n">
-        <v>0.1585105366541772</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Run_3</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.4513697606641847</v>
-      </c>
-      <c r="C4" t="n">
-        <v>6.685733939987119</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="n">
-        <v>0.1542344144691047</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0.1572230677642351</v>
-      </c>
-      <c r="W4" t="n">
-        <v>11.93727193906693</v>
-      </c>
-      <c r="X4" t="n">
-        <v>0.370794015024756</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>0.1627383979100372</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>6.695859030077964</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>0.07181160530642126</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>0.5661125649301948</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>7.233615393877918</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>0.1249113472238536</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>0.1581156293972831</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>1.442936931247835</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>-109.2343850968029</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>-107.6508661583468</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>0.2133285069480693</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>0.03064924132524034</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>6.827420823567663</v>
-      </c>
-      <c r="AL4" t="inlineStr"/>
-      <c r="AM4" t="inlineStr"/>
-      <c r="AN4" t="inlineStr"/>
-      <c r="AO4" t="inlineStr"/>
-      <c r="AP4" t="inlineStr"/>
-      <c r="AQ4" t="inlineStr"/>
-      <c r="AR4" t="n">
-        <v>206.1838520375338</v>
-      </c>
-      <c r="AS4" t="inlineStr"/>
-      <c r="AT4" t="inlineStr"/>
-      <c r="AU4" t="inlineStr"/>
-      <c r="AV4" t="inlineStr"/>
-      <c r="AW4" t="n">
-        <v>430026.4548396987</v>
-      </c>
-      <c r="AX4" t="inlineStr"/>
-      <c r="AY4" t="inlineStr"/>
+        <v>2350319.829006001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updating files v3, new general main
</commit_message>
<xml_diff>
--- a/Excel_Results/YX_C pH_UL.xlsx
+++ b/Excel_Results/YX_C pH_UL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM3"/>
+  <dimension ref="A1:AQ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Run</t>
+          <t>Model_</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -446,187 +446,207 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>YX_N_value</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Xmax_value</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>pH_UL_value</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>RMSE_X_og</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_X_og</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>MAPE_X_og</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>RMSE_C_og</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_C_og</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>MAPE_C_og</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>RMSE_N_og</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_N_og</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>MAPE_N_og</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>RMSE_pH_og</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_pH_og</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>MAPE_pH_og</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>AIC_og</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>BIC_og</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>RMSE_og</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_og</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>MAPE_og</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>RMSE_X_new</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_X_new</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>MAPE_X_new</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>RMSE_C_new</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_C_new</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>MAPE_C_new</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>RMSE_N_new</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_N_new</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>MAPE_N_new</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>RMSE_pH_new</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_pH_new</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>MAPE_pH_new</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>AIC_new</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>BIC_new</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>RMSE_new</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_new</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>MAPE_new</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>t_value_YX_C</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>t_value_pH_UL</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_YX_N</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_Xmax</t>
         </is>
       </c>
     </row>
@@ -640,61 +660,65 @@
         <v>0.484</v>
       </c>
       <c r="C2" t="n">
+        <v>21.575</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.4462</v>
+      </c>
+      <c r="E2" t="n">
         <v>7.4</v>
       </c>
-      <c r="D2" t="n">
+      <c r="F2" t="n">
         <v>0.2005851692302318</v>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
         <v>0.2044719770418198</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>17.90493789151974</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>0.3615215812803811</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>0.1586688041433045</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>6.02365418992219</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>0.06423696915458403</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
         <v>0.5063994213229439</v>
       </c>
-      <c r="L2" t="n">
+      <c r="N2" t="n">
         <v>6.51281349533272</v>
       </c>
-      <c r="M2" t="n">
+      <c r="O2" t="n">
         <v>0.1260098929727701</v>
       </c>
-      <c r="N2" t="n">
+      <c r="P2" t="n">
         <v>0.1595061936364179</v>
       </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
         <v>1.44764375959904</v>
       </c>
-      <c r="P2" t="n">
+      <c r="R2" t="n">
         <v>-81.51579256556585</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="S2" t="n">
         <v>-59.34652742718031</v>
       </c>
-      <c r="R2" t="n">
+      <c r="T2" t="n">
         <v>0.2184817756586141</v>
       </c>
-      <c r="S2" t="n">
+      <c r="U2" t="n">
         <v>0.03138961952683599</v>
       </c>
-      <c r="T2" t="n">
+      <c r="V2" t="n">
         <v>7.972262334093423</v>
       </c>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
@@ -712,21 +736,29 @@
       <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Run_3</t>
+          <t>Model2</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3019000248478971</v>
+        <v>0.5337722631906598</v>
       </c>
       <c r="C3" t="n">
-        <v>6.270094823160237</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+        <v>9.999999817378523</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.299999993866745</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7.298276094730486</v>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -742,62 +774,664 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
-      <c r="U3" t="n">
-        <v>0.1767723542181233</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0.1801977329232616</v>
-      </c>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
       <c r="W3" t="n">
-        <v>21.53459878428799</v>
+        <v>0.1666950775283088</v>
       </c>
       <c r="X3" t="n">
-        <v>1.288233347656097</v>
+        <v>0.1699251853771428</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.5653948624759768</v>
+        <v>12.7573052852034</v>
       </c>
       <c r="Z3" t="n">
-        <v>27.81498117706033</v>
+        <v>0.4973966127457704</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.05908581434424913</v>
+        <v>0.2183032212068513</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.4657913127924631</v>
+        <v>9.503372153709657</v>
       </c>
       <c r="AC3" t="n">
-        <v>5.922211725760993</v>
+        <v>0.04124121423891117</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.0780941576563732</v>
+        <v>0.3251169427838708</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.09885336412199139</v>
+        <v>4.011719538141475</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.9373952689530096</v>
+        <v>0.1382042806153576</v>
       </c>
       <c r="AG3" t="n">
-        <v>-28.79586067230095</v>
+        <v>0.1749421273612122</v>
       </c>
       <c r="AH3" t="n">
-        <v>-27.21234173384484</v>
+        <v>1.443995197679715</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.6519937603508629</v>
+        <v>-91.733831815283</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.0936729665876723</v>
+        <v>-90.15031287682689</v>
       </c>
       <c r="AK3" t="n">
-        <v>14.05229673901558</v>
+        <v>0.2720256882058397</v>
       </c>
       <c r="AL3" t="n">
-        <v>650.6571407306653</v>
+        <v>0.03908235745781009</v>
       </c>
       <c r="AM3" t="n">
-        <v>2350319.829006001</v>
+        <v>6.92909804368356</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>170.5200024179385</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>40499.63259207078</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>953.8697674829283</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>5897.430568617629</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Model3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.5337243187528518</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9.999900869725129</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.299999970085617</v>
+      </c>
+      <c r="E4" t="n">
+        <v>7.297871633242628</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="n">
+        <v>0.1667579358580045</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.169989261734312</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>12.76620411301375</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.4976142727513994</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0.2183987503663573</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>9.508686427151607</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.04125630551635923</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.3252359118801295</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>4.013450062069931</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0.1382576055590038</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0.1750096272898782</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>1.444599062324511</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>-91.7030104510609</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>-90.1194915126048</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0.2721421603947534</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0.03909909119994687</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>6.93323491613995</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>170.5006463463327</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>40381.57201193638</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>953.5111835337057</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>5888.572706380934</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Model4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5338533314985728</v>
+      </c>
+      <c r="C5" t="n">
+        <v>9.999828119557998</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.299999999214557</v>
+      </c>
+      <c r="E5" t="n">
+        <v>7.298381183461025</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="n">
+        <v>0.166678743179981</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.1699085345125297</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>12.75498672752157</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.4974506512621792</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0.2183269382606048</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>9.505166698821929</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.04123638666530649</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0.3250788855636754</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>4.011154298583155</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0.1381904017792491</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>0.1749245592142394</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>1.443837906152202</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>-91.72847093523345</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>-90.14495199677734</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0.2720459430860646</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0.03908526750823376</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>6.928786407769713</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>170.5031333019629</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>40530.34296989901</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>953.9819726043011</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>5899.736190793962</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Model5</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.5335030171522892</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9.999974624209445</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.299999984313408</v>
+      </c>
+      <c r="E6" t="n">
+        <v>7.298003916317391</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="n">
+        <v>0.1667374397316046</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.1699683684474216</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>12.76330900586245</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.4971610280051452</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0.2181998250307862</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>9.495975556346801</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.04125159417401379</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.3251987709460415</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>4.012912569127552</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0.1382402490499264</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0.1749876570252232</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>1.444402623804708</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>-91.75930642986361</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>-90.1757874914075</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>0.2719294587088104</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.03906853201497896</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>6.929149938785378</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>170.5826449108356</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>40420.07788406897</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>953.6233441909753</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>5891.446644710201</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Model6</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5337147905057675</v>
+      </c>
+      <c r="C7" t="n">
+        <v>9.999910577334287</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.299999995750383</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7.298183802487871</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="n">
+        <v>0.1667094255598719</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.1699398114354483</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>12.75933996189242</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.4973712694402341</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0.2182920982416102</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>9.50243091123488</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.0412443628409935</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.3251417641646652</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>4.012076764401371</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0.1382164649311847</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>0.1749575505458034</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>1.444133245415988</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>-91.73587508681442</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>-90.15235614835831</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>0.2720179685605922</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>0.03908124836426455</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>6.929495220736165</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>170.5304378975921</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>40472.6697106081</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>953.793967963884</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>5895.406013484932</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Model7</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.5337834550056796</v>
+      </c>
+      <c r="C8" t="n">
+        <v>9.999953073098444</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.299999998007177</v>
+      </c>
+      <c r="E8" t="n">
+        <v>7.298296256531162</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="n">
+        <v>0.166691944408292</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.1699219915455819</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>12.75686078913869</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.4973999487050964</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0.2183046853315518</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>9.503514573550255</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0.04124022602789235</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.3251091524180634</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>4.011603181436782</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0.138201619262022</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>0.1749387585595215</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>1.443965040937522</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>-91.73365461589248</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>-90.15013567743637</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>0.2720263576898047</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>0.0390824536436218</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>6.928985896265813</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>170.5181575435128</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>40505.52250812629</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>953.8926429800543</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>5897.87244510927</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Model8</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5337984219866544</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9.999996085732288</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.299999998126475</v>
+      </c>
+      <c r="E9" t="n">
+        <v>7.298348117199334</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="n">
+        <v>0.1666838907950994</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.1699137818747566</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>12.75571800036166</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0.4973862520810319</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0.2182986739975855</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>9.503241302178211</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0.0412384269062795</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.3250949693992251</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>4.011398630318967</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>0.138194778768046</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>0.1749300997063873</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>1.44388752065293</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>-91.73588639092344</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>-90.15236745246733</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>0.2720179258533627</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>0.03908124222844986</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>6.928561363377943</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>170.5178232740601</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>40520.66733198448</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>953.9357353701289</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>5899.007885543564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>